<commit_message>
alteracao para que todos os produtos fiquem na mesma linha do arquivo excel
</commit_message>
<xml_diff>
--- a/021-integracaoTxtPdf/08-mentoria-leituraXmlENotasfiscais/NFs.xlsx
+++ b/021-integracaoTxtPdf/08-mentoria-leituraXmlENotasfiscais/NFs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,217 +496,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>('b.box led', '389.00')</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>374.17</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>36882195000279</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>BROTA COMPANY COMERCIO DE PLANTAS LTDA</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>10000000000</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Lira da Hashtag</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>('Tomilho Serpilho', '10.00')</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>374.17</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>36882195000279</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>BROTA COMPANY COMERCIO DE PLANTAS LTDA</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>10000000000</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Lira da Hashtag</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>('Oregano Bravo-Europeu', '10.00')</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>374.17</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>36882195000279</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>BROTA COMPANY COMERCIO DE PLANTAS LTDA</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>10000000000</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Lira da Hashtag</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>('Manjericao Italiano', '10.00')</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>374.17</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>36882195000279</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>BROTA COMPANY COMERCIO DE PLANTAS LTDA</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>10000000000</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Lira da Hashtag</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>('Coentro Portugues', '10.00')</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>374.17</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>36882195000279</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>BROTA COMPANY COMERCIO DE PLANTAS LTDA</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>10000000000</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Lira da Hashtag</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>('Salsa Hortense', '10.00')</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>374.17</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>36882195000279</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>BROTA COMPANY COMERCIO DE PLANTAS LTDA</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>10000000000</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Lira da Hashtag</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>('Alface Baby-Leaf', '10.00')</t>
+          <t>[('b.box led', '389.00'), ('Tomilho Serpilho', '10.00'), ('Oregano Bravo-Europeu', '10.00'), ('Manjericao Italiano', '10.00'), ('Coentro Portugues', '10.00'), ('Salsa Hortense', '10.00'), ('Alface Baby-Leaf', '10.00')]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
finalizacao exercicio xml NFs
</commit_message>
<xml_diff>
--- a/021-integracaoTxtPdf/08-mentoria-leituraXmlENotasfiscais/NFs.xlsx
+++ b/021-integracaoTxtPdf/08-mentoria-leituraXmlENotasfiscais/NFs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>CNPJ Vendedor</t>
+          <t>CNPJ do Vendedor</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -471,32 +471,102 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>374.17</t>
+          <t>['374.17']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>36882195000279</t>
+          <t>['36882195000279']</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>BROTA COMPANY COMERCIO DE PLANTAS LTDA</t>
+          <t>['BROTA COMPANY COMERCIO DE PLANTAS LTDA']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>10000000000</t>
+          <t>['10000000000']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Lira da Hashtag</t>
+          <t>['Lira da Hashtag']</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[('b.box led', '389.00'), ('Tomilho Serpilho', '10.00'), ('Oregano Bravo-Europeu', '10.00'), ('Manjericao Italiano', '10.00'), ('Coentro Portugues', '10.00'), ('Salsa Hortense', '10.00'), ('Alface Baby-Leaf', '10.00')]</t>
+          <t>[[('b.box led', '389.00'), ('Tomilho Serpilho', '10.00'), ('Oregano Bravo-Europeu', '10.00'), ('Manjericao Italiano', '10.00'), ('Coentro Portugues', '10.00'), ('Salsa Hortense', '10.00'), ('Alface Baby-Leaf', '10.00')]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['849.00']</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['60409075055054']</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['NESTLE BRASIL LTDA']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>['11122233344']</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>['Lira da Hashtag']</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[[('ESSENZA Mini C30 Metal 110V', '534.82'), ('NOMAD Travel Mug Festve Medium', '104.35'), ('Pack YEP 2021 50 Caps OL', '130.00')]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['4500']</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>['30000000000101']</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['LIRA BOLADO NO XML']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>['26344392000108']</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>['HASHTAG TREINAMENTOS LTDA']</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['Nota referente aos serviços realizados no mês de Novembro de 2021.']</t>
         </is>
       </c>
     </row>

</xml_diff>